<commit_message>
update view and add students
</commit_message>
<xml_diff>
--- a/TatCaSinhVien_DiemHocPhan.xlsx
+++ b/TatCaSinhVien_DiemHocPhan.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,16 +484,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DTC1</t>
+          <t>DT3</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nguyễn Văn A</t>
+          <t>Dung</t>
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>36254</v>
+        <v>37350</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -502,37 +502,37 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Kinh</t>
+          <t>kinh</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Hà nội</t>
+          <t>Hà Tĩnh</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>CNTT_K17A</t>
+          <t>K17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DTC11</t>
+          <t>DTC1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Trần Thị D</t>
+          <t>Nguyễn Văn A</t>
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>35964</v>
+        <v>36254</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -542,32 +542,32 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Thái bình</t>
+          <t>Hà nội</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>QTVP_K16D</t>
+          <t>CNTT_K17A</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DTC12</t>
+          <t>DTC11</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Hoàng C</t>
+          <t>Trần Thị D</t>
         </is>
       </c>
       <c r="C4" s="1" t="n">
-        <v>36689</v>
+        <v>35964</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -577,28 +577,28 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Thái nguyên</t>
+          <t>Thái bình</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>CNTT_K17C</t>
+          <t>QTVP_K16D</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DTC15</t>
+          <t>DTC12</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sùng A C</t>
+          <t>Hoàng C</t>
         </is>
       </c>
       <c r="C5" s="1" t="n">
-        <v>35953</v>
+        <v>36689</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -607,68 +607,68 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Mông</t>
+          <t>Kinh</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Sơn la</t>
+          <t>Thái nguyên</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>KTPM_K15C</t>
+          <t>CNTT_K17C</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DTC18</t>
+          <t>DTC15</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Lò thị N</t>
+          <t>Sùng A C</t>
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>37031</v>
+        <v>35953</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Mường</t>
+          <t>Mông</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Lai châu</t>
+          <t>Sơn la</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>QTVP_K18E</t>
+          <t>KTPM_K15C</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DTC2</t>
+          <t>DTC18</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Hà Thị L</t>
+          <t>Lò thị N</t>
         </is>
       </c>
       <c r="C7" s="1" t="n">
-        <v>36323</v>
+        <v>37031</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -677,85 +677,155 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Thái</t>
+          <t>Mường</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Điện Biên</t>
+          <t>Lai châu</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>KTPM_K16C</t>
+          <t>QTVP_K18E</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DTC6</t>
+          <t>DTC2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Lường Minh H</t>
+          <t>Hà Thị L</t>
         </is>
       </c>
       <c r="C8" s="1" t="n">
-        <v>36324</v>
+        <v>36323</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Kinh</t>
+          <t>Thái</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Hà nội</t>
+          <t>Điện Biên</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>CNTT_K17C</t>
+          <t>KTPM_K16C</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>DTC5</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>37358</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Kinh</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Đà Nẵng</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>CNTT_K13B</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>DTC6</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Lường Minh H</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>36324</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Kinh</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Hà nội</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>CNTT_K17C</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>DTC8</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>Vi Vũ L</t>
         </is>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C11" s="1" t="n">
         <v>39612</v>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Nữ</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>Hài nhì</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>Lai châu</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>CNTT_K17A</t>
         </is>
@@ -772,7 +842,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -861,37 +931,37 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DTC1</t>
+          <t>DTC15</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Nguyễn Văn A</t>
+          <t>Sùng A C</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CNTT_K17A</t>
+          <t>KTPM_K15C</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>AV</t>
+          <t>ATTT</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Anh văn</t>
+          <t>An toàn và bảo mật thông tin</t>
         </is>
       </c>
       <c r="F3" t="n">
         <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H3" t="n">
-        <v>6</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="4">
@@ -912,94 +982,94 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CNTBM</t>
+          <t>AV</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Công nghệ và thiết bị mạng</t>
+          <t>Anh văn</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H4" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DTC1</t>
+          <t>DTC11</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Nguyễn Văn A</t>
+          <t>Trần Thị D</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CNTT_K17A</t>
+          <t>QTVP_K16D</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>LTW</t>
+          <t>AV</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Lập trình web</t>
+          <t>Anh văn</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H5" t="n">
-        <v>9</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DTC1</t>
+          <t>DTC18</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Nguyễn Văn A</t>
+          <t>Lò thị N</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CNTT_K17A</t>
+          <t>QTVP_K18E</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>QTH</t>
+          <t>AV</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Quản trị học</t>
+          <t>Anh văn</t>
         </is>
       </c>
       <c r="F6" t="n">
         <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>8.4</v>
       </c>
       <c r="H6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
@@ -1020,22 +1090,22 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>TTNT</t>
+          <t>CNTBM</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Trí tuệ nhân tạo</t>
+          <t>Công nghệ và thiết bị mạng</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7" t="n">
         <v>3</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -1056,38 +1126,38 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>AV</t>
+          <t>CNTBM</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Anh văn</t>
+          <t>Công nghệ và thiết bị mạng</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H8" t="n">
-        <v>7.5</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DTC11</t>
+          <t>DTC5</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Trần Thị D</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>QTVP_K16D</t>
+          <t>CNTT_K13B</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1104,98 +1174,98 @@
         <v>3</v>
       </c>
       <c r="G9" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H9" t="n">
-        <v>6.7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DTC11</t>
+          <t>DTC6</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Trần Thị D</t>
+          <t>Lường Minh H</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>QTVP_K16D</t>
+          <t>CNTT_K17C</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>LTW</t>
+          <t>CNTBM</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Lập trình web</t>
+          <t>Công nghệ và thiết bị mạng</t>
         </is>
       </c>
       <c r="F10" t="n">
         <v>3</v>
       </c>
       <c r="G10" t="n">
-        <v>9.800000000000001</v>
+        <v>7.5</v>
       </c>
       <c r="H10" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DTC11</t>
+          <t>DTC8</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Trần Thị D</t>
+          <t>Vi Vũ L</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>QTVP_K16D</t>
+          <t>CNTT_K17A</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>TCC1</t>
+          <t>CNTBM</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Toán cao cấp 1</t>
+          <t>Công nghệ và thiết bị mạng</t>
         </is>
       </c>
       <c r="F11" t="n">
         <v>3</v>
       </c>
       <c r="G11" t="n">
-        <v>7.8</v>
+        <v>5.5</v>
       </c>
       <c r="H11" t="n">
-        <v>6.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DTC12</t>
+          <t>DT3</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Hoàng C</t>
+          <t>Dung</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CNTT_K17C</t>
+          <t>K17</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1212,10 +1282,10 @@
         <v>3</v>
       </c>
       <c r="G12" t="n">
-        <v>9.300000000000001</v>
+        <v>4</v>
       </c>
       <c r="H12" t="n">
-        <v>8.199999999999999</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -1236,130 +1306,130 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>KCPM</t>
+          <t>CTDLTT</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Kiểm chứng phần mềm</t>
+          <t>Cấu trúc dữ liệu &amp; thuật toán</t>
         </is>
       </c>
       <c r="F13" t="n">
         <v>3</v>
       </c>
       <c r="G13" t="n">
-        <v>7.5</v>
+        <v>2</v>
       </c>
       <c r="H13" t="n">
-        <v>7.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>DTC15</t>
+          <t>DTC6</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Sùng A C</t>
+          <t>Lường Minh H</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>KTPM_K15C</t>
+          <t>CNTT_K17C</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ATTT</t>
+          <t>CTDLTT</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>An toàn và bảo mật thông tin</t>
+          <t>Cấu trúc dữ liệu &amp; thuật toán</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G14" t="n">
-        <v>7</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="H14" t="n">
-        <v>8.5</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>DTC15</t>
+          <t>DTC8</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sùng A C</t>
+          <t>Vi Vũ L</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>KTPM_K15C</t>
+          <t>CNTT_K17A</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>KCPM</t>
+          <t>CTDLTT</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Kiểm chứng phần mềm</t>
+          <t>Cấu trúc dữ liệu &amp; thuật toán</t>
         </is>
       </c>
       <c r="F15" t="n">
         <v>3</v>
       </c>
       <c r="G15" t="n">
-        <v>8.6</v>
+        <v>6</v>
       </c>
       <c r="H15" t="n">
-        <v>9</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DTC15</t>
+          <t>DTC12</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Sùng A C</t>
+          <t>Hoàng C</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>KTPM_K15C</t>
+          <t>CNTT_K17C</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>TCC1</t>
+          <t>KCPM</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Toán cao cấp 1</t>
+          <t>Kiểm chứng phần mềm</t>
         </is>
       </c>
       <c r="F16" t="n">
         <v>3</v>
       </c>
       <c r="G16" t="n">
-        <v>8.5</v>
+        <v>7.5</v>
       </c>
       <c r="H16" t="n">
-        <v>9.300000000000001</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="17">
@@ -1380,22 +1450,22 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>TTNT</t>
+          <t>KCPM</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Trí tuệ nhân tạo</t>
+          <t>Kiểm chứng phần mềm</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G17" t="n">
-        <v>5.5</v>
+        <v>8.6</v>
       </c>
       <c r="H17" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
@@ -1416,38 +1486,38 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>AV</t>
+          <t>KCPM</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Anh văn</t>
+          <t>Kiểm chứng phần mềm</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G18" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="H18" t="n">
         <v>8.4</v>
-      </c>
-      <c r="H18" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>DTC18</t>
+          <t>DTC2</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Lò thị N</t>
+          <t>Hà Thị L</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>QTVP_K18E</t>
+          <t>KTPM_K16C</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1464,187 +1534,187 @@
         <v>3</v>
       </c>
       <c r="G19" t="n">
-        <v>9.6</v>
+        <v>6.65</v>
       </c>
       <c r="H19" t="n">
-        <v>8.4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>DTC18</t>
+          <t>DTC8</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Lò thị N</t>
+          <t>Vi Vũ L</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>QTVP_K18E</t>
+          <t>CNTT_K17A</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>TCC2</t>
+          <t>KCPM</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Toán cao cấp 2</t>
+          <t>Kiểm chứng phần mềm</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G20" t="n">
-        <v>7.3</v>
+        <v>7</v>
       </c>
       <c r="H20" t="n">
-        <v>7.1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>DTC18</t>
+          <t>DTC1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Lò thị N</t>
+          <t>Nguyễn Văn A</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>QTVP_K18E</t>
+          <t>CNTT_K17A</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>TTNT</t>
+          <t>LTW</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Trí tuệ nhân tạo</t>
+          <t>Lập trình web</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G21" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H21" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>DTC2</t>
+          <t>DTC11</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Hà Thị L</t>
+          <t>Trần Thị D</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>KTPM_K16C</t>
+          <t>QTVP_K16D</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>KCPM</t>
+          <t>LTW</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Kiểm chứng phần mềm</t>
+          <t>Lập trình web</t>
         </is>
       </c>
       <c r="F22" t="n">
         <v>3</v>
       </c>
       <c r="G22" t="n">
-        <v>6.65</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H22" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>DTC2</t>
+          <t>DTC6</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Hà Thị L</t>
+          <t>Lường Minh H</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>KTPM_K16C</t>
+          <t>CNTT_K17C</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>QTH</t>
+          <t>LTW</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Quản trị học</t>
+          <t>Lập trình web</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G23" t="n">
-        <v>7</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="H23" t="n">
-        <v>7.8</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>DTC2</t>
+          <t>DTC8</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Hà Thị L</t>
+          <t>Vi Vũ L</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>KTPM_K16C</t>
+          <t>CNTT_K17A</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>TCC1</t>
+          <t>LTW</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Toán cao cấp 1</t>
+          <t>Lập trình web</t>
         </is>
       </c>
       <c r="F24" t="n">
         <v>3</v>
       </c>
       <c r="G24" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="H24" t="n">
         <v>5</v>
@@ -1653,34 +1723,34 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>DTC2</t>
+          <t>DTC1</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Hà Thị L</t>
+          <t>Nguyễn Văn A</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>KTPM_K16C</t>
+          <t>CNTT_K17A</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>TTNT</t>
+          <t>QTH</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Trí tuệ nhân tạo</t>
+          <t>Quản trị học</t>
         </is>
       </c>
       <c r="F25" t="n">
         <v>2</v>
       </c>
       <c r="G25" t="n">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="H25" t="n">
         <v>9</v>
@@ -1689,192 +1759,192 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>DTC6</t>
+          <t>DTC2</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Lường Minh H</t>
+          <t>Hà Thị L</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CNTT_K17C</t>
+          <t>KTPM_K16C</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>CNTBM</t>
+          <t>QTH</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Công nghệ và thiết bị mạng</t>
+          <t>Quản trị học</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G26" t="n">
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="H26" t="n">
-        <v>6</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>DTC6</t>
+          <t>DTC11</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Lường Minh H</t>
+          <t>Trần Thị D</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CNTT_K17C</t>
+          <t>QTVP_K16D</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>CTDLTT</t>
+          <t>TCC1</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Cấu trúc dữ liệu &amp; thuật toán</t>
+          <t>Toán cao cấp 1</t>
         </is>
       </c>
       <c r="F27" t="n">
         <v>3</v>
       </c>
       <c r="G27" t="n">
-        <v>9.300000000000001</v>
+        <v>7.8</v>
       </c>
       <c r="H27" t="n">
-        <v>8.1</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>DTC6</t>
+          <t>DTC15</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Lường Minh H</t>
+          <t>Sùng A C</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CNTT_K17C</t>
+          <t>KTPM_K15C</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>LTW</t>
+          <t>TCC1</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Lập trình web</t>
+          <t>Toán cao cấp 1</t>
         </is>
       </c>
       <c r="F28" t="n">
         <v>3</v>
       </c>
       <c r="G28" t="n">
-        <v>8.699999999999999</v>
+        <v>8.5</v>
       </c>
       <c r="H28" t="n">
-        <v>8.4</v>
+        <v>9.300000000000001</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>DTC8</t>
+          <t>DTC2</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Vi Vũ L</t>
+          <t>Hà Thị L</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CNTT_K17A</t>
+          <t>KTPM_K16C</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>CNTBM</t>
+          <t>TCC1</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Công nghệ và thiết bị mạng</t>
+          <t>Toán cao cấp 1</t>
         </is>
       </c>
       <c r="F29" t="n">
         <v>3</v>
       </c>
       <c r="G29" t="n">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="H29" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>DTC8</t>
+          <t>DTC18</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Vi Vũ L</t>
+          <t>Lò thị N</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>CNTT_K17A</t>
+          <t>QTVP_K18E</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>CTDLTT</t>
+          <t>TCC2</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Cấu trúc dữ liệu &amp; thuật toán</t>
+          <t>Toán cao cấp 2</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G30" t="n">
-        <v>6</v>
+        <v>7.3</v>
       </c>
       <c r="H30" t="n">
-        <v>6.5</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>DTC8</t>
+          <t>DTC1</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Vi Vũ L</t>
+          <t>Nguyễn Văn A</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1884,58 +1954,130 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>KCPM</t>
+          <t>TTNT</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Kiểm chứng phần mềm</t>
+          <t>Trí tuệ nhân tạo</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G31" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H31" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>DTC8</t>
+          <t>DTC15</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Vi Vũ L</t>
+          <t>Sùng A C</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>CNTT_K17A</t>
+          <t>KTPM_K15C</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>LTW</t>
+          <t>TTNT</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Lập trình web</t>
+          <t>Trí tuệ nhân tạo</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G32" t="n">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="H32" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>DTC18</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Lò thị N</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>QTVP_K18E</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>TTNT</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Trí tuệ nhân tạo</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" t="n">
         <v>5</v>
+      </c>
+      <c r="H33" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>DTC2</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Hà Thị L</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>KTPM_K16C</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>TTNT</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Trí tuệ nhân tạo</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>2</v>
+      </c>
+      <c r="G34" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="H34" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>